<commit_message>
mise à jour: Sprint2
</commit_message>
<xml_diff>
--- a/livrable1/Backlog.xlsx
+++ b/livrable1/Backlog.xlsx
@@ -1,20 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\louca\Documents\Cegep\Session6\ESP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp\www\ESP_repository\livrable1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5B3C1E8-DFCF-412A-8AF4-FB01DE4EAFBB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A333814C-81A3-4143-925A-38C6C0DEF57A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-7920" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Backlog" sheetId="1" r:id="rId1"/>
     <sheet name="Sprint1" sheetId="2" r:id="rId2"/>
+    <sheet name="Sprint2" sheetId="3" r:id="rId3"/>
+    <sheet name="Sprint3" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Tableau1[#All]</definedName>
@@ -37,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="32">
   <si>
     <t>ID</t>
   </si>
@@ -738,25 +740,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:J133"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="14.140625" customWidth="1"/>
+    <col min="2" max="2" width="14.1796875" customWidth="1"/>
     <col min="3" max="3" width="15" customWidth="1"/>
-    <col min="4" max="4" width="14.28515625" customWidth="1"/>
-    <col min="6" max="6" width="74.28515625" customWidth="1"/>
-    <col min="10" max="10" width="44.42578125" customWidth="1"/>
+    <col min="4" max="4" width="14.26953125" customWidth="1"/>
+    <col min="6" max="6" width="74.26953125" customWidth="1"/>
+    <col min="10" max="10" width="44.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:10" x14ac:dyDescent="0.35">
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
     </row>
-    <row r="3" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B3" s="9" t="s">
         <v>0</v>
       </c>
@@ -776,7 +778,7 @@
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
     </row>
-    <row r="4" spans="2:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:10" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B4" s="13">
         <v>1</v>
       </c>
@@ -794,7 +796,7 @@
       <c r="I4" s="1"/>
       <c r="J4" s="8"/>
     </row>
-    <row r="5" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B5" s="2"/>
       <c r="C5" s="4" t="s">
         <v>4</v>
@@ -808,7 +810,7 @@
       <c r="I5" s="1"/>
       <c r="J5" s="8"/>
     </row>
-    <row r="6" spans="2:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:10" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B6" s="16">
         <v>2</v>
       </c>
@@ -826,7 +828,7 @@
       <c r="I6" s="1"/>
       <c r="J6" s="8"/>
     </row>
-    <row r="7" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B7" s="2"/>
       <c r="C7" s="4" t="s">
         <v>4</v>
@@ -840,7 +842,7 @@
       <c r="I7" s="1"/>
       <c r="J7" s="8"/>
     </row>
-    <row r="8" spans="2:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:10" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B8" s="16">
         <v>3</v>
       </c>
@@ -858,7 +860,7 @@
       <c r="I8" s="1"/>
       <c r="J8" s="8"/>
     </row>
-    <row r="9" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B9" s="2"/>
       <c r="C9" s="4" t="s">
         <v>4</v>
@@ -872,7 +874,7 @@
       <c r="I9" s="1"/>
       <c r="J9" s="8"/>
     </row>
-    <row r="10" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B10" s="2"/>
       <c r="C10" s="4" t="s">
         <v>5</v>
@@ -886,7 +888,7 @@
       <c r="I10" s="1"/>
       <c r="J10" s="8"/>
     </row>
-    <row r="11" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B11" s="2"/>
       <c r="C11" s="4" t="s">
         <v>13</v>
@@ -900,7 +902,7 @@
       <c r="I11" s="1"/>
       <c r="J11" s="8"/>
     </row>
-    <row r="12" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B12" s="2"/>
       <c r="C12" s="4" t="s">
         <v>15</v>
@@ -914,7 +916,7 @@
       <c r="I12" s="1"/>
       <c r="J12" s="8"/>
     </row>
-    <row r="13" spans="2:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:10" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B13" s="14">
         <v>4</v>
       </c>
@@ -932,7 +934,7 @@
       <c r="I13" s="1"/>
       <c r="J13" s="8"/>
     </row>
-    <row r="14" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B14" s="2"/>
       <c r="C14" s="2" t="s">
         <v>4</v>
@@ -946,7 +948,7 @@
       <c r="I14" s="1"/>
       <c r="J14" s="8"/>
     </row>
-    <row r="15" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B15" s="2"/>
       <c r="C15" s="4" t="s">
         <v>5</v>
@@ -960,7 +962,7 @@
       <c r="I15" s="1"/>
       <c r="J15" s="8"/>
     </row>
-    <row r="16" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B16" s="2"/>
       <c r="C16" s="4" t="s">
         <v>13</v>
@@ -974,7 +976,7 @@
       <c r="I16" s="1"/>
       <c r="J16" s="8"/>
     </row>
-    <row r="17" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B17" s="2"/>
       <c r="C17" s="4" t="s">
         <v>15</v>
@@ -988,7 +990,7 @@
       <c r="I17" s="1"/>
       <c r="J17" s="8"/>
     </row>
-    <row r="18" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B18" s="5"/>
       <c r="C18" s="5" t="s">
         <v>22</v>
@@ -1002,7 +1004,7 @@
       <c r="I18" s="1"/>
       <c r="J18" s="8"/>
     </row>
-    <row r="19" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B19" s="2"/>
       <c r="C19" s="4" t="s">
         <v>23</v>
@@ -1016,7 +1018,7 @@
       <c r="I19" s="1"/>
       <c r="J19" s="8"/>
     </row>
-    <row r="20" spans="2:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:10" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B20" s="16">
         <v>5</v>
       </c>
@@ -1034,7 +1036,7 @@
       <c r="I20" s="1"/>
       <c r="J20" s="8"/>
     </row>
-    <row r="21" spans="2:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:10" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B21" s="16">
         <v>6</v>
       </c>
@@ -1052,7 +1054,7 @@
       <c r="I21" s="1"/>
       <c r="J21" s="8"/>
     </row>
-    <row r="22" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B22" s="2"/>
       <c r="C22" s="2" t="s">
         <v>4</v>
@@ -1066,7 +1068,7 @@
       <c r="I22" s="1"/>
       <c r="J22" s="8"/>
     </row>
-    <row r="23" spans="2:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:10" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B23" s="16">
         <v>7</v>
       </c>
@@ -1084,7 +1086,7 @@
       <c r="I23" s="1"/>
       <c r="J23" s="8"/>
     </row>
-    <row r="24" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B24" s="2"/>
       <c r="C24" s="4" t="s">
         <v>4</v>
@@ -1098,7 +1100,7 @@
       <c r="I24" s="1"/>
       <c r="J24" s="8"/>
     </row>
-    <row r="25" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B25" s="4"/>
       <c r="C25" s="4"/>
       <c r="D25" s="4"/>
@@ -1108,7 +1110,7 @@
       <c r="I25" s="1"/>
       <c r="J25" s="8"/>
     </row>
-    <row r="26" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B26" s="2"/>
       <c r="C26" s="4"/>
       <c r="D26" s="2"/>
@@ -1118,7 +1120,7 @@
       <c r="I26" s="1"/>
       <c r="J26" s="8"/>
     </row>
-    <row r="27" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B27" s="2"/>
       <c r="C27" s="4"/>
       <c r="D27" s="2"/>
@@ -1128,7 +1130,7 @@
       <c r="I27" s="1"/>
       <c r="J27" s="8"/>
     </row>
-    <row r="28" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B28" s="2"/>
       <c r="C28" s="4"/>
       <c r="D28" s="2"/>
@@ -1138,7 +1140,7 @@
       <c r="I28" s="1"/>
       <c r="J28" s="8"/>
     </row>
-    <row r="29" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B29" s="2"/>
       <c r="C29" s="4"/>
       <c r="D29" s="2"/>
@@ -1148,7 +1150,7 @@
       <c r="I29" s="1"/>
       <c r="J29" s="8"/>
     </row>
-    <row r="30" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B30" s="2"/>
       <c r="C30" s="4"/>
       <c r="D30" s="2"/>
@@ -1158,7 +1160,7 @@
       <c r="I30" s="1"/>
       <c r="J30" s="8"/>
     </row>
-    <row r="31" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B31" s="2"/>
       <c r="C31" s="4"/>
       <c r="D31" s="2"/>
@@ -1168,7 +1170,7 @@
       <c r="I31" s="1"/>
       <c r="J31" s="8"/>
     </row>
-    <row r="32" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B32" s="2"/>
       <c r="C32" s="4"/>
       <c r="D32" s="2"/>
@@ -1178,7 +1180,7 @@
       <c r="I32" s="1"/>
       <c r="J32" s="8"/>
     </row>
-    <row r="33" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B33" s="2"/>
       <c r="C33" s="4"/>
       <c r="D33" s="2"/>
@@ -1188,7 +1190,7 @@
       <c r="I33" s="1"/>
       <c r="J33" s="8"/>
     </row>
-    <row r="34" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B34" s="2"/>
       <c r="C34" s="4"/>
       <c r="D34" s="2"/>
@@ -1198,7 +1200,7 @@
       <c r="I34" s="1"/>
       <c r="J34" s="8"/>
     </row>
-    <row r="35" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B35" s="3"/>
       <c r="C35" s="5"/>
       <c r="D35" s="3"/>
@@ -1208,7 +1210,7 @@
       <c r="I35" s="1"/>
       <c r="J35" s="8"/>
     </row>
-    <row r="36" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B36" s="2"/>
       <c r="C36" s="4"/>
       <c r="D36" s="2"/>
@@ -1218,7 +1220,7 @@
       <c r="I36" s="1"/>
       <c r="J36" s="8"/>
     </row>
-    <row r="37" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B37" s="2"/>
       <c r="C37" s="4"/>
       <c r="D37" s="2"/>
@@ -1228,7 +1230,7 @@
       <c r="I37" s="1"/>
       <c r="J37" s="8"/>
     </row>
-    <row r="38" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B38" s="2"/>
       <c r="C38" s="4"/>
       <c r="D38" s="2"/>
@@ -1238,7 +1240,7 @@
       <c r="I38" s="1"/>
       <c r="J38" s="8"/>
     </row>
-    <row r="39" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B39" s="2"/>
       <c r="C39" s="4"/>
       <c r="D39" s="2"/>
@@ -1248,7 +1250,7 @@
       <c r="I39" s="1"/>
       <c r="J39" s="8"/>
     </row>
-    <row r="40" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B40" s="2"/>
       <c r="C40" s="4"/>
       <c r="D40" s="2"/>
@@ -1258,467 +1260,467 @@
       <c r="I40" s="1"/>
       <c r="J40" s="8"/>
     </row>
-    <row r="41" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:10" x14ac:dyDescent="0.35">
       <c r="E41" s="1"/>
       <c r="F41" s="1"/>
       <c r="H41" s="1"/>
       <c r="I41" s="1"/>
       <c r="J41" s="8"/>
     </row>
-    <row r="42" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:10" x14ac:dyDescent="0.35">
       <c r="G42" s="8"/>
     </row>
-    <row r="43" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:10" x14ac:dyDescent="0.35">
       <c r="H43" s="1"/>
       <c r="I43" s="1"/>
       <c r="J43" s="8"/>
     </row>
-    <row r="44" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:10" x14ac:dyDescent="0.35">
       <c r="H44" s="1"/>
       <c r="I44" s="1"/>
       <c r="J44" s="8"/>
     </row>
-    <row r="45" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:10" x14ac:dyDescent="0.35">
       <c r="H45" s="1"/>
       <c r="I45" s="1"/>
       <c r="J45" s="8"/>
     </row>
-    <row r="46" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:10" x14ac:dyDescent="0.35">
       <c r="H46" s="1"/>
       <c r="I46" s="1"/>
       <c r="J46" s="8"/>
     </row>
-    <row r="47" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:10" x14ac:dyDescent="0.35">
       <c r="H47" s="1"/>
       <c r="I47" s="1"/>
       <c r="J47" s="8"/>
     </row>
-    <row r="48" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:10" x14ac:dyDescent="0.35">
       <c r="H48" s="1"/>
       <c r="I48" s="1"/>
       <c r="J48" s="8"/>
     </row>
-    <row r="49" spans="8:10" x14ac:dyDescent="0.25">
+    <row r="49" spans="8:10" x14ac:dyDescent="0.35">
       <c r="H49" s="1"/>
       <c r="I49" s="1"/>
       <c r="J49" s="8"/>
     </row>
-    <row r="50" spans="8:10" x14ac:dyDescent="0.25">
+    <row r="50" spans="8:10" x14ac:dyDescent="0.35">
       <c r="H50" s="1"/>
       <c r="I50" s="1"/>
       <c r="J50" s="1"/>
     </row>
-    <row r="51" spans="8:10" x14ac:dyDescent="0.25">
+    <row r="51" spans="8:10" x14ac:dyDescent="0.35">
       <c r="H51" s="1"/>
       <c r="I51" s="1"/>
       <c r="J51" s="1"/>
     </row>
-    <row r="52" spans="8:10" x14ac:dyDescent="0.25">
+    <row r="52" spans="8:10" x14ac:dyDescent="0.35">
       <c r="H52" s="1"/>
       <c r="I52" s="1"/>
       <c r="J52" s="1"/>
     </row>
-    <row r="53" spans="8:10" x14ac:dyDescent="0.25">
+    <row r="53" spans="8:10" x14ac:dyDescent="0.35">
       <c r="H53" s="1"/>
       <c r="I53" s="1"/>
       <c r="J53" s="1"/>
     </row>
-    <row r="54" spans="8:10" x14ac:dyDescent="0.25">
+    <row r="54" spans="8:10" x14ac:dyDescent="0.35">
       <c r="H54" s="1"/>
       <c r="I54" s="1"/>
       <c r="J54" s="1"/>
     </row>
-    <row r="55" spans="8:10" x14ac:dyDescent="0.25">
+    <row r="55" spans="8:10" x14ac:dyDescent="0.35">
       <c r="H55" s="1"/>
       <c r="I55" s="1"/>
       <c r="J55" s="1"/>
     </row>
-    <row r="56" spans="8:10" x14ac:dyDescent="0.25">
+    <row r="56" spans="8:10" x14ac:dyDescent="0.35">
       <c r="H56" s="1"/>
       <c r="I56" s="1"/>
       <c r="J56" s="1"/>
     </row>
-    <row r="57" spans="8:10" x14ac:dyDescent="0.25">
+    <row r="57" spans="8:10" x14ac:dyDescent="0.35">
       <c r="H57" s="1"/>
       <c r="I57" s="1"/>
       <c r="J57" s="1"/>
     </row>
-    <row r="58" spans="8:10" x14ac:dyDescent="0.25">
+    <row r="58" spans="8:10" x14ac:dyDescent="0.35">
       <c r="H58" s="1"/>
       <c r="I58" s="1"/>
       <c r="J58" s="1"/>
     </row>
-    <row r="59" spans="8:10" x14ac:dyDescent="0.25">
+    <row r="59" spans="8:10" x14ac:dyDescent="0.35">
       <c r="H59" s="1"/>
       <c r="I59" s="1"/>
       <c r="J59" s="1"/>
     </row>
-    <row r="60" spans="8:10" x14ac:dyDescent="0.25">
+    <row r="60" spans="8:10" x14ac:dyDescent="0.35">
       <c r="H60" s="1"/>
       <c r="I60" s="1"/>
       <c r="J60" s="1"/>
     </row>
-    <row r="61" spans="8:10" x14ac:dyDescent="0.25">
+    <row r="61" spans="8:10" x14ac:dyDescent="0.35">
       <c r="H61" s="1"/>
       <c r="I61" s="1"/>
       <c r="J61" s="1"/>
     </row>
-    <row r="62" spans="8:10" x14ac:dyDescent="0.25">
+    <row r="62" spans="8:10" x14ac:dyDescent="0.35">
       <c r="H62" s="1"/>
       <c r="I62" s="1"/>
       <c r="J62" s="1"/>
     </row>
-    <row r="63" spans="8:10" x14ac:dyDescent="0.25">
+    <row r="63" spans="8:10" x14ac:dyDescent="0.35">
       <c r="H63" s="1"/>
       <c r="I63" s="1"/>
       <c r="J63" s="1"/>
     </row>
-    <row r="64" spans="8:10" x14ac:dyDescent="0.25">
+    <row r="64" spans="8:10" x14ac:dyDescent="0.35">
       <c r="H64" s="1"/>
       <c r="I64" s="1"/>
       <c r="J64" s="1"/>
     </row>
-    <row r="65" spans="8:10" x14ac:dyDescent="0.25">
+    <row r="65" spans="8:10" x14ac:dyDescent="0.35">
       <c r="H65" s="1"/>
       <c r="I65" s="1"/>
       <c r="J65" s="1"/>
     </row>
-    <row r="66" spans="8:10" x14ac:dyDescent="0.25">
+    <row r="66" spans="8:10" x14ac:dyDescent="0.35">
       <c r="H66" s="1"/>
       <c r="I66" s="1"/>
       <c r="J66" s="1"/>
     </row>
-    <row r="67" spans="8:10" x14ac:dyDescent="0.25">
+    <row r="67" spans="8:10" x14ac:dyDescent="0.35">
       <c r="H67" s="1"/>
       <c r="I67" s="1"/>
       <c r="J67" s="1"/>
     </row>
-    <row r="68" spans="8:10" x14ac:dyDescent="0.25">
+    <row r="68" spans="8:10" x14ac:dyDescent="0.35">
       <c r="H68" s="1"/>
       <c r="I68" s="1"/>
       <c r="J68" s="1"/>
     </row>
-    <row r="69" spans="8:10" x14ac:dyDescent="0.25">
+    <row r="69" spans="8:10" x14ac:dyDescent="0.35">
       <c r="H69" s="1"/>
       <c r="I69" s="1"/>
       <c r="J69" s="1"/>
     </row>
-    <row r="70" spans="8:10" x14ac:dyDescent="0.25">
+    <row r="70" spans="8:10" x14ac:dyDescent="0.35">
       <c r="H70" s="1"/>
       <c r="I70" s="1"/>
       <c r="J70" s="1"/>
     </row>
-    <row r="71" spans="8:10" x14ac:dyDescent="0.25">
+    <row r="71" spans="8:10" x14ac:dyDescent="0.35">
       <c r="H71" s="1"/>
       <c r="I71" s="1"/>
       <c r="J71" s="1"/>
     </row>
-    <row r="72" spans="8:10" x14ac:dyDescent="0.25">
+    <row r="72" spans="8:10" x14ac:dyDescent="0.35">
       <c r="H72" s="1"/>
       <c r="I72" s="1"/>
       <c r="J72" s="1"/>
     </row>
-    <row r="73" spans="8:10" x14ac:dyDescent="0.25">
+    <row r="73" spans="8:10" x14ac:dyDescent="0.35">
       <c r="H73" s="1"/>
       <c r="I73" s="1"/>
       <c r="J73" s="1"/>
     </row>
-    <row r="74" spans="8:10" x14ac:dyDescent="0.25">
+    <row r="74" spans="8:10" x14ac:dyDescent="0.35">
       <c r="H74" s="1"/>
       <c r="I74" s="1"/>
       <c r="J74" s="1"/>
     </row>
-    <row r="75" spans="8:10" x14ac:dyDescent="0.25">
+    <row r="75" spans="8:10" x14ac:dyDescent="0.35">
       <c r="H75" s="1"/>
       <c r="I75" s="1"/>
       <c r="J75" s="1"/>
     </row>
-    <row r="76" spans="8:10" x14ac:dyDescent="0.25">
+    <row r="76" spans="8:10" x14ac:dyDescent="0.35">
       <c r="H76" s="1"/>
       <c r="I76" s="1"/>
       <c r="J76" s="1"/>
     </row>
-    <row r="77" spans="8:10" x14ac:dyDescent="0.25">
+    <row r="77" spans="8:10" x14ac:dyDescent="0.35">
       <c r="H77" s="1"/>
       <c r="I77" s="1"/>
       <c r="J77" s="1"/>
     </row>
-    <row r="78" spans="8:10" x14ac:dyDescent="0.25">
+    <row r="78" spans="8:10" x14ac:dyDescent="0.35">
       <c r="H78" s="1"/>
       <c r="I78" s="1"/>
       <c r="J78" s="1"/>
     </row>
-    <row r="79" spans="8:10" x14ac:dyDescent="0.25">
+    <row r="79" spans="8:10" x14ac:dyDescent="0.35">
       <c r="H79" s="1"/>
       <c r="I79" s="1"/>
       <c r="J79" s="1"/>
     </row>
-    <row r="80" spans="8:10" x14ac:dyDescent="0.25">
+    <row r="80" spans="8:10" x14ac:dyDescent="0.35">
       <c r="H80" s="1"/>
       <c r="I80" s="1"/>
       <c r="J80" s="1"/>
     </row>
-    <row r="81" spans="8:10" x14ac:dyDescent="0.25">
+    <row r="81" spans="8:10" x14ac:dyDescent="0.35">
       <c r="H81" s="1"/>
       <c r="I81" s="1"/>
       <c r="J81" s="1"/>
     </row>
-    <row r="82" spans="8:10" x14ac:dyDescent="0.25">
+    <row r="82" spans="8:10" x14ac:dyDescent="0.35">
       <c r="H82" s="1"/>
       <c r="I82" s="1"/>
       <c r="J82" s="1"/>
     </row>
-    <row r="83" spans="8:10" x14ac:dyDescent="0.25">
+    <row r="83" spans="8:10" x14ac:dyDescent="0.35">
       <c r="H83" s="1"/>
       <c r="I83" s="1"/>
       <c r="J83" s="1"/>
     </row>
-    <row r="84" spans="8:10" x14ac:dyDescent="0.25">
+    <row r="84" spans="8:10" x14ac:dyDescent="0.35">
       <c r="H84" s="1"/>
       <c r="I84" s="1"/>
       <c r="J84" s="1"/>
     </row>
-    <row r="85" spans="8:10" x14ac:dyDescent="0.25">
+    <row r="85" spans="8:10" x14ac:dyDescent="0.35">
       <c r="H85" s="1"/>
       <c r="I85" s="1"/>
       <c r="J85" s="1"/>
     </row>
-    <row r="86" spans="8:10" x14ac:dyDescent="0.25">
+    <row r="86" spans="8:10" x14ac:dyDescent="0.35">
       <c r="H86" s="1"/>
       <c r="I86" s="1"/>
       <c r="J86" s="1"/>
     </row>
-    <row r="87" spans="8:10" x14ac:dyDescent="0.25">
+    <row r="87" spans="8:10" x14ac:dyDescent="0.35">
       <c r="H87" s="1"/>
       <c r="I87" s="1"/>
       <c r="J87" s="1"/>
     </row>
-    <row r="88" spans="8:10" x14ac:dyDescent="0.25">
+    <row r="88" spans="8:10" x14ac:dyDescent="0.35">
       <c r="H88" s="1"/>
       <c r="I88" s="1"/>
       <c r="J88" s="1"/>
     </row>
-    <row r="89" spans="8:10" x14ac:dyDescent="0.25">
+    <row r="89" spans="8:10" x14ac:dyDescent="0.35">
       <c r="H89" s="1"/>
       <c r="I89" s="1"/>
       <c r="J89" s="1"/>
     </row>
-    <row r="90" spans="8:10" x14ac:dyDescent="0.25">
+    <row r="90" spans="8:10" x14ac:dyDescent="0.35">
       <c r="H90" s="1"/>
       <c r="I90" s="1"/>
       <c r="J90" s="1"/>
     </row>
-    <row r="91" spans="8:10" x14ac:dyDescent="0.25">
+    <row r="91" spans="8:10" x14ac:dyDescent="0.35">
       <c r="H91" s="1"/>
       <c r="I91" s="1"/>
       <c r="J91" s="1"/>
     </row>
-    <row r="92" spans="8:10" x14ac:dyDescent="0.25">
+    <row r="92" spans="8:10" x14ac:dyDescent="0.35">
       <c r="H92" s="1"/>
       <c r="I92" s="1"/>
       <c r="J92" s="1"/>
     </row>
-    <row r="93" spans="8:10" x14ac:dyDescent="0.25">
+    <row r="93" spans="8:10" x14ac:dyDescent="0.35">
       <c r="H93" s="1"/>
       <c r="I93" s="1"/>
       <c r="J93" s="1"/>
     </row>
-    <row r="94" spans="8:10" x14ac:dyDescent="0.25">
+    <row r="94" spans="8:10" x14ac:dyDescent="0.35">
       <c r="H94" s="1"/>
       <c r="I94" s="1"/>
       <c r="J94" s="1"/>
     </row>
-    <row r="95" spans="8:10" x14ac:dyDescent="0.25">
+    <row r="95" spans="8:10" x14ac:dyDescent="0.35">
       <c r="H95" s="1"/>
       <c r="I95" s="1"/>
       <c r="J95" s="1"/>
     </row>
-    <row r="96" spans="8:10" x14ac:dyDescent="0.25">
+    <row r="96" spans="8:10" x14ac:dyDescent="0.35">
       <c r="H96" s="1"/>
       <c r="I96" s="1"/>
       <c r="J96" s="1"/>
     </row>
-    <row r="97" spans="8:10" x14ac:dyDescent="0.25">
+    <row r="97" spans="8:10" x14ac:dyDescent="0.35">
       <c r="H97" s="1"/>
       <c r="I97" s="1"/>
       <c r="J97" s="1"/>
     </row>
-    <row r="98" spans="8:10" x14ac:dyDescent="0.25">
+    <row r="98" spans="8:10" x14ac:dyDescent="0.35">
       <c r="H98" s="1"/>
       <c r="I98" s="1"/>
       <c r="J98" s="1"/>
     </row>
-    <row r="99" spans="8:10" x14ac:dyDescent="0.25">
+    <row r="99" spans="8:10" x14ac:dyDescent="0.35">
       <c r="H99" s="1"/>
       <c r="I99" s="1"/>
       <c r="J99" s="1"/>
     </row>
-    <row r="100" spans="8:10" x14ac:dyDescent="0.25">
+    <row r="100" spans="8:10" x14ac:dyDescent="0.35">
       <c r="H100" s="1"/>
       <c r="I100" s="1"/>
       <c r="J100" s="1"/>
     </row>
-    <row r="101" spans="8:10" x14ac:dyDescent="0.25">
+    <row r="101" spans="8:10" x14ac:dyDescent="0.35">
       <c r="H101" s="1"/>
       <c r="I101" s="1"/>
       <c r="J101" s="1"/>
     </row>
-    <row r="102" spans="8:10" x14ac:dyDescent="0.25">
+    <row r="102" spans="8:10" x14ac:dyDescent="0.35">
       <c r="H102" s="1"/>
       <c r="I102" s="1"/>
       <c r="J102" s="1"/>
     </row>
-    <row r="103" spans="8:10" x14ac:dyDescent="0.25">
+    <row r="103" spans="8:10" x14ac:dyDescent="0.35">
       <c r="H103" s="1"/>
       <c r="I103" s="1"/>
       <c r="J103" s="1"/>
     </row>
-    <row r="104" spans="8:10" x14ac:dyDescent="0.25">
+    <row r="104" spans="8:10" x14ac:dyDescent="0.35">
       <c r="H104" s="1"/>
       <c r="I104" s="1"/>
       <c r="J104" s="1"/>
     </row>
-    <row r="105" spans="8:10" x14ac:dyDescent="0.25">
+    <row r="105" spans="8:10" x14ac:dyDescent="0.35">
       <c r="H105" s="1"/>
       <c r="I105" s="1"/>
       <c r="J105" s="1"/>
     </row>
-    <row r="106" spans="8:10" x14ac:dyDescent="0.25">
+    <row r="106" spans="8:10" x14ac:dyDescent="0.35">
       <c r="H106" s="1"/>
       <c r="I106" s="1"/>
       <c r="J106" s="1"/>
     </row>
-    <row r="107" spans="8:10" x14ac:dyDescent="0.25">
+    <row r="107" spans="8:10" x14ac:dyDescent="0.35">
       <c r="H107" s="1"/>
       <c r="I107" s="1"/>
       <c r="J107" s="1"/>
     </row>
-    <row r="108" spans="8:10" x14ac:dyDescent="0.25">
+    <row r="108" spans="8:10" x14ac:dyDescent="0.35">
       <c r="H108" s="1"/>
       <c r="I108" s="1"/>
       <c r="J108" s="1"/>
     </row>
-    <row r="109" spans="8:10" x14ac:dyDescent="0.25">
+    <row r="109" spans="8:10" x14ac:dyDescent="0.35">
       <c r="H109" s="1"/>
       <c r="I109" s="1"/>
       <c r="J109" s="1"/>
     </row>
-    <row r="110" spans="8:10" x14ac:dyDescent="0.25">
+    <row r="110" spans="8:10" x14ac:dyDescent="0.35">
       <c r="H110" s="1"/>
       <c r="I110" s="1"/>
       <c r="J110" s="1"/>
     </row>
-    <row r="111" spans="8:10" x14ac:dyDescent="0.25">
+    <row r="111" spans="8:10" x14ac:dyDescent="0.35">
       <c r="H111" s="1"/>
       <c r="I111" s="1"/>
       <c r="J111" s="1"/>
     </row>
-    <row r="112" spans="8:10" x14ac:dyDescent="0.25">
+    <row r="112" spans="8:10" x14ac:dyDescent="0.35">
       <c r="H112" s="1"/>
       <c r="I112" s="1"/>
       <c r="J112" s="1"/>
     </row>
-    <row r="113" spans="8:10" x14ac:dyDescent="0.25">
+    <row r="113" spans="8:10" x14ac:dyDescent="0.35">
       <c r="H113" s="1"/>
       <c r="I113" s="1"/>
       <c r="J113" s="1"/>
     </row>
-    <row r="114" spans="8:10" x14ac:dyDescent="0.25">
+    <row r="114" spans="8:10" x14ac:dyDescent="0.35">
       <c r="H114" s="1"/>
       <c r="I114" s="1"/>
       <c r="J114" s="1"/>
     </row>
-    <row r="115" spans="8:10" x14ac:dyDescent="0.25">
+    <row r="115" spans="8:10" x14ac:dyDescent="0.35">
       <c r="H115" s="1"/>
       <c r="I115" s="1"/>
       <c r="J115" s="1"/>
     </row>
-    <row r="116" spans="8:10" x14ac:dyDescent="0.25">
+    <row r="116" spans="8:10" x14ac:dyDescent="0.35">
       <c r="H116" s="1"/>
       <c r="I116" s="1"/>
       <c r="J116" s="1"/>
     </row>
-    <row r="117" spans="8:10" x14ac:dyDescent="0.25">
+    <row r="117" spans="8:10" x14ac:dyDescent="0.35">
       <c r="H117" s="1"/>
       <c r="I117" s="1"/>
       <c r="J117" s="1"/>
     </row>
-    <row r="118" spans="8:10" x14ac:dyDescent="0.25">
+    <row r="118" spans="8:10" x14ac:dyDescent="0.35">
       <c r="H118" s="1"/>
       <c r="I118" s="1"/>
       <c r="J118" s="1"/>
     </row>
-    <row r="119" spans="8:10" x14ac:dyDescent="0.25">
+    <row r="119" spans="8:10" x14ac:dyDescent="0.35">
       <c r="H119" s="1"/>
       <c r="I119" s="1"/>
       <c r="J119" s="1"/>
     </row>
-    <row r="120" spans="8:10" x14ac:dyDescent="0.25">
+    <row r="120" spans="8:10" x14ac:dyDescent="0.35">
       <c r="H120" s="1"/>
       <c r="I120" s="1"/>
       <c r="J120" s="1"/>
     </row>
-    <row r="121" spans="8:10" x14ac:dyDescent="0.25">
+    <row r="121" spans="8:10" x14ac:dyDescent="0.35">
       <c r="H121" s="1"/>
       <c r="I121" s="1"/>
       <c r="J121" s="1"/>
     </row>
-    <row r="122" spans="8:10" x14ac:dyDescent="0.25">
+    <row r="122" spans="8:10" x14ac:dyDescent="0.35">
       <c r="H122" s="1"/>
       <c r="I122" s="1"/>
       <c r="J122" s="1"/>
     </row>
-    <row r="123" spans="8:10" x14ac:dyDescent="0.25">
+    <row r="123" spans="8:10" x14ac:dyDescent="0.35">
       <c r="H123" s="1"/>
       <c r="I123" s="1"/>
       <c r="J123" s="1"/>
     </row>
-    <row r="124" spans="8:10" x14ac:dyDescent="0.25">
+    <row r="124" spans="8:10" x14ac:dyDescent="0.35">
       <c r="H124" s="1"/>
       <c r="I124" s="1"/>
       <c r="J124" s="1"/>
     </row>
-    <row r="125" spans="8:10" x14ac:dyDescent="0.25">
+    <row r="125" spans="8:10" x14ac:dyDescent="0.35">
       <c r="H125" s="1"/>
       <c r="I125" s="1"/>
       <c r="J125" s="1"/>
     </row>
-    <row r="126" spans="8:10" x14ac:dyDescent="0.25">
+    <row r="126" spans="8:10" x14ac:dyDescent="0.35">
       <c r="H126" s="1"/>
       <c r="I126" s="1"/>
       <c r="J126" s="1"/>
     </row>
-    <row r="127" spans="8:10" x14ac:dyDescent="0.25">
+    <row r="127" spans="8:10" x14ac:dyDescent="0.35">
       <c r="H127" s="1"/>
       <c r="I127" s="1"/>
       <c r="J127" s="1"/>
     </row>
-    <row r="128" spans="8:10" x14ac:dyDescent="0.25">
+    <row r="128" spans="8:10" x14ac:dyDescent="0.35">
       <c r="H128" s="1"/>
       <c r="I128" s="1"/>
       <c r="J128" s="1"/>
     </row>
-    <row r="129" spans="8:10" x14ac:dyDescent="0.25">
+    <row r="129" spans="8:10" x14ac:dyDescent="0.35">
       <c r="H129" s="1"/>
       <c r="I129" s="1"/>
       <c r="J129" s="1"/>
     </row>
-    <row r="130" spans="8:10" x14ac:dyDescent="0.25">
+    <row r="130" spans="8:10" x14ac:dyDescent="0.35">
       <c r="H130" s="1"/>
       <c r="I130" s="1"/>
       <c r="J130" s="1"/>
     </row>
-    <row r="131" spans="8:10" x14ac:dyDescent="0.25">
+    <row r="131" spans="8:10" x14ac:dyDescent="0.35">
       <c r="H131" s="1"/>
       <c r="I131" s="1"/>
       <c r="J131" s="1"/>
     </row>
-    <row r="132" spans="8:10" x14ac:dyDescent="0.25">
+    <row r="132" spans="8:10" x14ac:dyDescent="0.35">
       <c r="H132" s="1"/>
       <c r="I132" s="1"/>
       <c r="J132" s="1"/>
     </row>
-    <row r="133" spans="8:10" x14ac:dyDescent="0.25">
+    <row r="133" spans="8:10" x14ac:dyDescent="0.35">
       <c r="H133" s="1"/>
       <c r="I133" s="1"/>
       <c r="J133" s="1"/>
@@ -1737,19 +1739,19 @@
   <dimension ref="B1:F16"/>
   <sheetViews>
     <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="9.7109375" customWidth="1"/>
-    <col min="4" max="4" width="15.140625" customWidth="1"/>
-    <col min="5" max="5" width="22.140625" customWidth="1"/>
+    <col min="3" max="3" width="9.7265625" customWidth="1"/>
+    <col min="4" max="4" width="15.1796875" customWidth="1"/>
+    <col min="5" max="5" width="22.1796875" customWidth="1"/>
     <col min="6" max="6" width="49" customWidth="1"/>
-    <col min="7" max="7" width="12.85546875" customWidth="1"/>
+    <col min="7" max="7" width="12.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:6" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B1" s="20" t="s">
         <v>0</v>
       </c>
@@ -1766,7 +1768,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="2:6" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B2" s="17">
         <v>5</v>
       </c>
@@ -1781,7 +1783,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="2:6" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B3" s="17">
         <v>7</v>
       </c>
@@ -1796,7 +1798,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B4" s="4"/>
       <c r="C4" s="4" t="s">
         <v>4</v>
@@ -1807,12 +1809,301 @@
         <v>28</v>
       </c>
     </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:6" x14ac:dyDescent="0.35">
       <c r="C16" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D01EFAC-69B6-496B-919A-A282DA3B3371}">
+  <dimension ref="B1:F15"/>
+  <sheetViews>
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="5" max="5" width="10.90625" customWidth="1"/>
+    <col min="6" max="6" width="88.08984375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B1" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="21" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="2:6" ht="32.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B2" s="14">
+        <v>4</v>
+      </c>
+      <c r="C2" s="14"/>
+      <c r="D2" s="13">
+        <v>1</v>
+      </c>
+      <c r="E2" s="13">
+        <v>40</v>
+      </c>
+      <c r="F2" s="19" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B3" s="4"/>
+      <c r="C3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B4" s="4"/>
+      <c r="C4" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="23" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B5" s="4"/>
+      <c r="C5" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="23" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B6" s="4"/>
+      <c r="C6" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="23" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B7" s="5"/>
+      <c r="C7" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="12" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B8" s="4"/>
+      <c r="C8" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="23" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B9" s="14">
+        <v>1</v>
+      </c>
+      <c r="C9" s="14"/>
+      <c r="D9" s="13">
+        <v>2</v>
+      </c>
+      <c r="E9" s="13">
+        <v>32</v>
+      </c>
+      <c r="F9" s="19" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B10" s="4"/>
+      <c r="C10" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="23" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B11" s="17">
+        <v>3</v>
+      </c>
+      <c r="C11" s="17"/>
+      <c r="D11" s="16">
+        <v>3</v>
+      </c>
+      <c r="E11" s="16">
+        <v>24</v>
+      </c>
+      <c r="F11" s="22" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B12" s="4"/>
+      <c r="C12" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="23" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B13" s="4"/>
+      <c r="C13" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="23" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B14" s="4"/>
+      <c r="C14" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="23" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B15" s="4"/>
+      <c r="C15" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="23" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCCAACF9-E5D6-44F3-AC6D-06E07E4ABBFC}">
+  <dimension ref="B1:F5"/>
+  <sheetViews>
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="6" max="6" width="70.26953125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B1" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="21" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="2:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B2" s="17">
+        <v>2</v>
+      </c>
+      <c r="C2" s="17"/>
+      <c r="D2" s="16">
+        <v>1</v>
+      </c>
+      <c r="E2" s="16">
+        <v>24</v>
+      </c>
+      <c r="F2" s="22" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B3" s="4"/>
+      <c r="C3" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="23" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B4" s="17">
+        <v>6</v>
+      </c>
+      <c r="C4" s="17"/>
+      <c r="D4" s="16">
+        <v>2</v>
+      </c>
+      <c r="E4" s="16">
+        <v>16</v>
+      </c>
+      <c r="F4" s="22" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B5" s="4"/>
+      <c r="C5" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="23" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -1975,6 +2266,12 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -1983,20 +2280,37 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{78A72A8A-1150-49A3-91CA-ADF2CD5833A4}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{78A72A8A-1150-49A3-91CA-ADF2CD5833A4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="76671e3e-87f0-403f-9dfb-f64b8a8298e6"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{89122351-3C00-47AC-9F02-4F277E314F97}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1C86C245-0F2A-47EC-B13B-CFC9EEB07458}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1C86C245-0F2A-47EC-B13B-CFC9EEB07458}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{89122351-3C00-47AC-9F02-4F277E314F97}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
continuer interface pour sprite 2 et modifier backlog pour sprint 2
</commit_message>
<xml_diff>
--- a/livrable1/Backlog.xlsx
+++ b/livrable1/Backlog.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp\www\ESP_repository\livrable1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A333814C-81A3-4143-925A-38C6C0DEF57A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67A73A7D-3D04-4F3A-A37D-ACF20FB06104}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-7920" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-7920" windowWidth="25440" windowHeight="15390" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Backlog" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="37">
   <si>
     <t>ID</t>
   </si>
@@ -135,6 +135,21 @@
   </si>
   <si>
     <t>En tant qu'administrateur je souhaite conserver les informations de production dans un base de donnée afin de les sauvegarder</t>
+  </si>
+  <si>
+    <t>En tant qu'utilisateur je souhaite avoir des graphiques afin de mieux interpréter les données.</t>
+  </si>
+  <si>
+    <t>Les tableaux doit être fait en chart.js</t>
+  </si>
+  <si>
+    <t>Un graphique pour la température</t>
+  </si>
+  <si>
+    <t>Un graphique pour l'humidité</t>
+  </si>
+  <si>
+    <t>Le graphique doit être mis à jour en direct</t>
   </si>
 </sst>
 </file>
@@ -740,8 +755,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:J133"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1100,52 +1115,76 @@
       <c r="I24" s="1"/>
       <c r="J24" s="8"/>
     </row>
-    <row r="25" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B25" s="4"/>
-      <c r="C25" s="4"/>
-      <c r="D25" s="4"/>
-      <c r="E25" s="4"/>
-      <c r="F25" s="4"/>
+    <row r="25" spans="2:10" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B25" s="17">
+        <v>8</v>
+      </c>
+      <c r="C25" s="17"/>
+      <c r="D25" s="16">
+        <v>4</v>
+      </c>
+      <c r="E25" s="16">
+        <v>20</v>
+      </c>
+      <c r="F25" s="22" t="s">
+        <v>32</v>
+      </c>
       <c r="H25" s="1"/>
       <c r="I25" s="1"/>
       <c r="J25" s="8"/>
     </row>
     <row r="26" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B26" s="2"/>
-      <c r="C26" s="4"/>
+      <c r="B26" s="4"/>
+      <c r="C26" s="4" t="s">
+        <v>4</v>
+      </c>
       <c r="D26" s="2"/>
       <c r="E26" s="2"/>
-      <c r="F26" s="7"/>
+      <c r="F26" s="23" t="s">
+        <v>33</v>
+      </c>
       <c r="H26" s="1"/>
       <c r="I26" s="1"/>
       <c r="J26" s="8"/>
     </row>
     <row r="27" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B27" s="2"/>
-      <c r="C27" s="4"/>
+      <c r="B27" s="4"/>
+      <c r="C27" s="4" t="s">
+        <v>5</v>
+      </c>
       <c r="D27" s="2"/>
       <c r="E27" s="2"/>
-      <c r="F27" s="7"/>
+      <c r="F27" s="23" t="s">
+        <v>34</v>
+      </c>
       <c r="H27" s="1"/>
       <c r="I27" s="1"/>
       <c r="J27" s="8"/>
     </row>
     <row r="28" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B28" s="2"/>
-      <c r="C28" s="4"/>
+      <c r="B28" s="4"/>
+      <c r="C28" s="4" t="s">
+        <v>13</v>
+      </c>
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
-      <c r="F28" s="7"/>
+      <c r="F28" s="23" t="s">
+        <v>35</v>
+      </c>
       <c r="H28" s="1"/>
       <c r="I28" s="1"/>
       <c r="J28" s="8"/>
     </row>
     <row r="29" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B29" s="2"/>
-      <c r="C29" s="4"/>
+      <c r="B29" s="4"/>
+      <c r="C29" s="4" t="s">
+        <v>15</v>
+      </c>
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>
-      <c r="F29" s="7"/>
+      <c r="F29" s="23" t="s">
+        <v>36</v>
+      </c>
       <c r="H29" s="1"/>
       <c r="I29" s="1"/>
       <c r="J29" s="8"/>
@@ -1820,10 +1859,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D01EFAC-69B6-496B-919A-A282DA3B3371}">
-  <dimension ref="B1:F15"/>
+  <dimension ref="B1:F20"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1858,7 +1897,7 @@
         <v>1</v>
       </c>
       <c r="E2" s="13">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="F2" s="19" t="s">
         <v>26</v>
@@ -1939,7 +1978,7 @@
         <v>2</v>
       </c>
       <c r="E9" s="13">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="F9" s="19" t="s">
         <v>7</v>
@@ -1965,7 +2004,7 @@
         <v>3</v>
       </c>
       <c r="E11" s="16">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F11" s="22" t="s">
         <v>9</v>
@@ -2013,6 +2052,65 @@
       <c r="E15" s="2"/>
       <c r="F15" s="23" t="s">
         <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B16" s="17">
+        <v>8</v>
+      </c>
+      <c r="C16" s="17"/>
+      <c r="D16" s="16">
+        <v>4</v>
+      </c>
+      <c r="E16" s="16">
+        <v>20</v>
+      </c>
+      <c r="F16" s="22" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B17" s="4"/>
+      <c r="C17" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="23" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B18" s="4"/>
+      <c r="C18" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="23" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B19" s="4"/>
+      <c r="C19" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="23" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B20" s="4"/>
+      <c r="C20" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="23" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -2025,7 +2123,7 @@
   <dimension ref="B1:F5"/>
   <sheetViews>
     <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2085,7 +2183,7 @@
         <v>2</v>
       </c>
       <c r="E4" s="16">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="F4" s="22" t="s">
         <v>29</v>
@@ -2108,6 +2206,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100E68C16B78B101B489C32F7F7C71E1B6E" ma:contentTypeVersion="6" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="55fb80f6f40a1e30ed82b9a221612fea">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="76671e3e-87f0-403f-9dfb-f64b8a8298e6" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="468c69a32aba556b96a81b67e4f81cc7" ns2:_="">
     <xsd:import namespace="76671e3e-87f0-403f-9dfb-f64b8a8298e6"/>
@@ -2265,22 +2378,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{89122351-3C00-47AC-9F02-4F277E314F97}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1C86C245-0F2A-47EC-B13B-CFC9EEB07458}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{78A72A8A-1150-49A3-91CA-ADF2CD5833A4}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2296,21 +2411,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1C86C245-0F2A-47EC-B13B-CFC9EEB07458}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{89122351-3C00-47AC-9F02-4F277E314F97}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
back log sprint 3
</commit_message>
<xml_diff>
--- a/livrable1/Backlog.xlsx
+++ b/livrable1/Backlog.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp\www\ESP_repository\livrable1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\ESP_repository\livrable1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67A73A7D-3D04-4F3A-A37D-ACF20FB06104}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FC133A2-BEA7-4ACC-A085-A331BE74FFEB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-7920" windowWidth="25440" windowHeight="15390" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-7920" windowWidth="25440" windowHeight="15390" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Backlog" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="39">
   <si>
     <t>ID</t>
   </si>
@@ -150,6 +150,12 @@
   </si>
   <si>
     <t>Le graphique doit être mis à jour en direct</t>
+  </si>
+  <si>
+    <t>La cause de l'arrêt de la machine doit être afficher.</t>
+  </si>
+  <si>
+    <t>Le message disparait après que l'utilisateur ai cliquer sur "ok"</t>
   </si>
 </sst>
 </file>
@@ -165,7 +171,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -181,6 +187,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -269,7 +281,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -310,6 +322,16 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -755,7 +777,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:J133"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView topLeftCell="A4" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
@@ -1861,7 +1883,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D01EFAC-69B6-496B-919A-A282DA3B3371}">
   <dimension ref="B1:F20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
@@ -2120,10 +2142,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCCAACF9-E5D6-44F3-AC6D-06E07E4ABBFC}">
-  <dimension ref="B1:F5"/>
+  <dimension ref="B1:F10"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2138,67 +2160,118 @@
       <c r="C1" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="21" t="s">
+      <c r="D1" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="21" t="s">
+      <c r="E1" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="F1" s="21" t="s">
+      <c r="F1" s="20" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="2:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B2" s="17">
+      <c r="B2" s="14">
         <v>2</v>
       </c>
-      <c r="C2" s="17"/>
-      <c r="D2" s="16">
+      <c r="C2" s="14"/>
+      <c r="D2" s="14">
         <v>1</v>
       </c>
-      <c r="E2" s="16">
+      <c r="E2" s="14">
         <v>24</v>
       </c>
-      <c r="F2" s="22" t="s">
+      <c r="F2" s="24" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="3" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B3" s="4"/>
-      <c r="C3" s="4" t="s">
+      <c r="B3" s="5"/>
+      <c r="C3" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="23" t="s">
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="25" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="2:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B4" s="17">
+    <row r="4" spans="2:6" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B4" s="26"/>
+      <c r="C4" s="26" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="26"/>
+      <c r="E4" s="26"/>
+      <c r="F4" s="27" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" ht="14.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B5" s="5"/>
+      <c r="C5" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B6" s="14">
         <v>6</v>
       </c>
-      <c r="C4" s="17"/>
-      <c r="D4" s="16">
+      <c r="C6" s="14"/>
+      <c r="D6" s="14">
         <v>2</v>
       </c>
-      <c r="E4" s="16">
+      <c r="E6" s="14">
         <v>20</v>
       </c>
-      <c r="F4" s="22" t="s">
+      <c r="F6" s="24" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B5" s="4"/>
-      <c r="C5" s="2" t="s">
+    <row r="7" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B7" s="5"/>
+      <c r="C7" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="23" t="s">
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="25" t="s">
         <v>8</v>
       </c>
+    </row>
+    <row r="8" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B8" s="5"/>
+      <c r="C8" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="27" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B9" s="5"/>
+      <c r="C9" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B10" s="5"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2206,21 +2279,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100E68C16B78B101B489C32F7F7C71E1B6E" ma:contentTypeVersion="6" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="55fb80f6f40a1e30ed82b9a221612fea">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="76671e3e-87f0-403f-9dfb-f64b8a8298e6" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="468c69a32aba556b96a81b67e4f81cc7" ns2:_="">
     <xsd:import namespace="76671e3e-87f0-403f-9dfb-f64b8a8298e6"/>
@@ -2378,24 +2436,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{89122351-3C00-47AC-9F02-4F277E314F97}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1C86C245-0F2A-47EC-B13B-CFC9EEB07458}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{78A72A8A-1150-49A3-91CA-ADF2CD5833A4}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2411,4 +2467,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1C86C245-0F2A-47EC-B13B-CFC9EEB07458}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{89122351-3C00-47AC-9F02-4F277E314F97}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>